<commit_message>
Finished signoff for available rooms
Moved ROOMS31 to No Error Files.  See remark in signoff
</commit_message>
<xml_diff>
--- a/TestFiles/Test files for availableRooms/FileIndex.xlsx
+++ b/TestFiles/Test files for availableRooms/FileIndex.xlsx
@@ -237,7 +237,7 @@
     <t>ROOMS31</t>
   </si>
   <si>
-    <t>Duplicate room names on line one and two.</t>
+    <t>Duplicate room names on line one and two. Input is accepted.</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>